<commit_message>
Problem 2 Mathemetical Formulation
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 03/AMPL Models/Model Setup.xlsx
+++ b/03 - Homework/HW 03/AMPL Models/Model Setup.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/03 - Homework/HW 03/AMPL Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="874" documentId="8_{F9186C4A-4D24-4C11-A94A-4E97A374E8E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6F0D1871-18DA-414B-951F-368227AA7017}"/>
+  <xr:revisionPtr revIDLastSave="1245" documentId="8_{F9186C4A-4D24-4C11-A94A-4E97A374E8E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{59BD5A0E-1C08-4C88-A7B9-F6BFDFD38855}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2581705E-783A-44E8-BFE7-0D5AB3EE4BE1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2581705E-783A-44E8-BFE7-0D5AB3EE4BE1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Problem 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Problem 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="97">
   <si>
     <t>A</t>
   </si>
@@ -298,18 +299,6 @@
     </r>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Period</t>
   </si>
   <si>
@@ -866,17 +855,489 @@
   </si>
   <si>
     <t>F needs to be per period per business</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+  </si>
+  <si>
+    <t>p in PRODUCTS</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Silo 1</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Silo 2</t>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+  </si>
+  <si>
+    <t>Silo 3</t>
+  </si>
+  <si>
+    <t>Silo 4</t>
+  </si>
+  <si>
+    <t>Silo 5</t>
+  </si>
+  <si>
+    <t>Silo 6</t>
+  </si>
+  <si>
+    <t>Silo 7</t>
+  </si>
+  <si>
+    <t>Silo 8</t>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+  </si>
+  <si>
+    <t>Total Capacity over all Silos</t>
+  </si>
+  <si>
+    <t>Total Supply of Products over all Products</t>
+  </si>
+  <si>
+    <t>Supply of Products</t>
+  </si>
+  <si>
+    <t>Supply (Tons)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Problem 1 Assumption: Partially filling tanks is fine, i.e. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">supply of product </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>capacity of the silos</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cost of Storing Product p in Silo s </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Cost per Ton)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total Silo Capacity - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Demand </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(Tons) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="2" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>capacity</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1" tint="0.39997558519241921"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>supply</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p</t>
+    </r>
+  </si>
+  <si>
+    <t>Can only store one type of product in each silo</t>
+  </si>
+  <si>
+    <t>Decision Variables</t>
+  </si>
+  <si>
+    <r>
+      <t>tonsOfProduct</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">p,s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Amount of product p to store in silo s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>isStored</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Binary variable </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SUM{p in PRODUCTS}(tonsOfProduct</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) &lt;= M</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> * SUM{p in PRODUCTS}(isStored</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p,s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>What is put in the silo must only be from one product</t>
+  </si>
+  <si>
+    <t>Supplied Product &lt;= capacity of the silo</t>
+  </si>
+  <si>
+    <t>Supplied Product == the total available product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="#,##0&quot; tons&quot;"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,8 +1444,96 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1051,8 +1600,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBE5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1328,11 +1911,111 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5" tint="0.39994506668294322"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1395,30 +2078,82 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="14" fillId="14" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="14" fillId="13" borderId="22" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="41" fontId="14" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="14" fillId="17" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="14" fillId="17" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDEBE5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1729,8 +2464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43754CE3-6374-400F-883E-506732118FF2}">
   <dimension ref="B1:S33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1749,19 +2484,19 @@
   <sheetData>
     <row r="1" spans="2:19" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
@@ -1780,12 +2515,15 @@
         <v>14</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:19" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>8</v>
@@ -1800,21 +2538,21 @@
         <v>9</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="O3" s="40"/>
+      <c r="L3" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="35"/>
       <c r="P3" s="14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="14"/>
       <c r="R3" s="14"/>
@@ -1822,7 +2560,7 @@
     </row>
     <row r="4" spans="2:19" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>3</v>
@@ -1837,52 +2575,52 @@
         <v>6</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="N4" s="39" t="str">
+      <c r="L4" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="34" t="str">
         <f t="shared" ref="N4:O4" si="0">L4</f>
         <v>Period 1</v>
       </c>
-      <c r="O4" s="39" t="str">
+      <c r="O4" s="34" t="str">
         <f t="shared" si="0"/>
         <v>Period 2</v>
       </c>
-      <c r="P4" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="R4" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="S4" s="36" t="s">
-        <v>53</v>
+      <c r="P4" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q4" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="31" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="38">
         <v>3000</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="38">
         <v>700</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="37">
         <v>5</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <v>2100</v>
       </c>
       <c r="H5" s="18">
@@ -1905,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="22">
-        <f t="shared" ref="O5:O8" si="1">M5 * $E5</f>
+        <f t="shared" ref="O5:O7" si="1">M5 * $E5</f>
         <v>10500</v>
       </c>
       <c r="P5" s="22">
@@ -1920,7 +2658,7 @@
         <f>D5 * COUNTIFS(L5:M5,  "&gt;0")</f>
         <v>700</v>
       </c>
-      <c r="S5" s="37">
+      <c r="S5" s="32">
         <f>SUM(P5:R5)</f>
         <v>14200</v>
       </c>
@@ -1929,16 +2667,16 @@
       <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="39">
         <v>2000</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="39">
         <v>500</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="39">
         <v>4</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="41">
         <v>1800</v>
       </c>
       <c r="H6" s="19">
@@ -1957,7 +2695,7 @@
         <v>1800</v>
       </c>
       <c r="N6" s="22">
-        <f t="shared" ref="N6:N8" si="3">L6 * $E6</f>
+        <f t="shared" ref="N6:N7" si="3">L6 * $E6</f>
         <v>0</v>
       </c>
       <c r="O6" s="22">
@@ -1976,7 +2714,7 @@
         <f t="shared" ref="R6:R7" si="5">D6 * COUNTIFS(L6:M6,  "&gt;0")</f>
         <v>500</v>
       </c>
-      <c r="S6" s="37">
+      <c r="S6" s="32">
         <f t="shared" ref="S6:S8" si="6">SUM(P6:R6)</f>
         <v>9700</v>
       </c>
@@ -1985,16 +2723,16 @@
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="40">
         <v>1000</v>
       </c>
-      <c r="D7" s="34">
+      <c r="D7" s="40">
         <v>900</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="40">
         <v>7</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="42">
         <v>3000</v>
       </c>
       <c r="K7" t="s">
@@ -2026,63 +2764,57 @@
         <f t="shared" si="5"/>
         <v>900</v>
       </c>
-      <c r="S7" s="37">
+      <c r="S7" s="32">
         <f t="shared" si="6"/>
         <v>22200</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
-        <v>53</v>
-      </c>
-      <c r="L8" s="41">
+        <v>49</v>
+      </c>
+      <c r="L8" s="36">
         <f>SUM(L5:L7)</f>
         <v>2900</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="36">
         <f>SUM(M5:M7)</f>
         <v>3900</v>
       </c>
-      <c r="N8" s="41">
+      <c r="N8" s="36">
         <f>SUM(N5:N7)</f>
         <v>20300</v>
       </c>
-      <c r="O8" s="41">
+      <c r="O8" s="36">
         <f>SUM(O5:O7)</f>
         <v>17700</v>
       </c>
-      <c r="P8" s="38">
+      <c r="P8" s="33">
         <f t="shared" si="4"/>
         <v>38000</v>
       </c>
-      <c r="Q8" s="38">
+      <c r="Q8" s="33">
         <f>SUM(Q5:Q7)</f>
         <v>6000</v>
       </c>
-      <c r="R8" s="38">
+      <c r="R8" s="33">
         <f>SUM(R5:R7)</f>
         <v>2100</v>
       </c>
-      <c r="S8" s="38">
+      <c r="S8" s="33">
         <f t="shared" si="6"/>
         <v>46100</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="F9" s="22">
-        <f>SUM(F5:F7)</f>
-        <v>6900</v>
-      </c>
-      <c r="I9" s="22">
-        <f>SUM(I5:I6)</f>
-        <v>6800</v>
-      </c>
+      <c r="F9" s="22"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F10" s="22"/>
       <c r="I10" s="22"/>
       <c r="R10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
@@ -2094,33 +2826,33 @@
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F12" s="22"/>
       <c r="I12" s="22"/>
       <c r="R12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F13" s="22"/>
       <c r="I13" s="22"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F14" s="22"/>
       <c r="I14" s="22"/>
@@ -2134,7 +2866,7 @@
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="28" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16">
@@ -2144,10 +2876,10 @@
     </row>
     <row r="17" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B17" s="23" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2160,10 +2892,10 @@
     </row>
     <row r="18" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -2172,54 +2904,54 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:9" collapsed="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B27" s="24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
@@ -2227,10 +2959,10 @@
     </row>
     <row r="28" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" s="24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="25"/>
@@ -2238,10 +2970,10 @@
     </row>
     <row r="29" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B29" s="24" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
@@ -2278,4 +3010,603 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71F040E-57EE-4CA4-8D4D-1306A72BE7E8}">
+  <dimension ref="B1:M45"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" s="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="M2" s="52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="10"/>
+      <c r="M3" s="53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="M4" s="54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="48">
+        <v>1</v>
+      </c>
+      <c r="D5" s="48">
+        <v>2</v>
+      </c>
+      <c r="E5" s="48">
+        <v>2</v>
+      </c>
+      <c r="F5" s="48">
+        <v>1</v>
+      </c>
+      <c r="G5" s="48">
+        <v>4</v>
+      </c>
+      <c r="H5" s="48">
+        <v>4</v>
+      </c>
+      <c r="I5" s="48">
+        <v>5</v>
+      </c>
+      <c r="J5" s="49">
+        <v>3</v>
+      </c>
+      <c r="K5" s="63"/>
+      <c r="M5" s="49">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="39">
+        <v>2</v>
+      </c>
+      <c r="D6" s="39">
+        <v>3</v>
+      </c>
+      <c r="E6" s="39">
+        <v>3</v>
+      </c>
+      <c r="F6" s="39">
+        <v>3</v>
+      </c>
+      <c r="G6" s="39">
+        <v>1</v>
+      </c>
+      <c r="H6" s="39">
+        <v>4</v>
+      </c>
+      <c r="I6" s="39">
+        <v>5</v>
+      </c>
+      <c r="J6" s="41">
+        <v>2</v>
+      </c>
+      <c r="K6" s="63"/>
+      <c r="M6" s="41">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="39">
+        <v>3</v>
+      </c>
+      <c r="D7" s="39">
+        <v>4</v>
+      </c>
+      <c r="E7" s="39">
+        <v>1</v>
+      </c>
+      <c r="F7" s="39">
+        <v>2</v>
+      </c>
+      <c r="G7" s="39">
+        <v>1</v>
+      </c>
+      <c r="H7" s="39">
+        <v>4</v>
+      </c>
+      <c r="I7" s="39">
+        <v>5</v>
+      </c>
+      <c r="J7" s="41">
+        <v>1</v>
+      </c>
+      <c r="K7" s="63"/>
+      <c r="M7" s="41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="39">
+        <v>1</v>
+      </c>
+      <c r="D8" s="39">
+        <v>1</v>
+      </c>
+      <c r="E8" s="39">
+        <v>2</v>
+      </c>
+      <c r="F8" s="39">
+        <v>2</v>
+      </c>
+      <c r="G8" s="39">
+        <v>3</v>
+      </c>
+      <c r="H8" s="39">
+        <v>4</v>
+      </c>
+      <c r="I8" s="39">
+        <v>5</v>
+      </c>
+      <c r="J8" s="41">
+        <v>2</v>
+      </c>
+      <c r="K8" s="63"/>
+      <c r="M8" s="41">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="40">
+        <v>1</v>
+      </c>
+      <c r="D9" s="40">
+        <v>1</v>
+      </c>
+      <c r="E9" s="40">
+        <v>1</v>
+      </c>
+      <c r="F9" s="40">
+        <v>1</v>
+      </c>
+      <c r="G9" s="40">
+        <v>1</v>
+      </c>
+      <c r="H9" s="40">
+        <v>1</v>
+      </c>
+      <c r="I9" s="40">
+        <v>5</v>
+      </c>
+      <c r="J9" s="42">
+        <v>5</v>
+      </c>
+      <c r="K9" s="63"/>
+      <c r="M9" s="42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+    </row>
+    <row r="11" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B11" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="50">
+        <v>25</v>
+      </c>
+      <c r="D11" s="50">
+        <v>25</v>
+      </c>
+      <c r="E11" s="50">
+        <v>30</v>
+      </c>
+      <c r="F11" s="50">
+        <v>60</v>
+      </c>
+      <c r="G11" s="50">
+        <v>80</v>
+      </c>
+      <c r="H11" s="50">
+        <v>85</v>
+      </c>
+      <c r="I11" s="50">
+        <v>100</v>
+      </c>
+      <c r="J11" s="50">
+        <v>50</v>
+      </c>
+      <c r="K11" s="60"/>
+    </row>
+    <row r="13" spans="2:13" ht="18" x14ac:dyDescent="0.35">
+      <c r="B13" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="62">
+        <f t="shared" ref="C13:J13" si="0">C11 + 1</f>
+        <v>26</v>
+      </c>
+      <c r="D13" s="62">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E13" s="62">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F13" s="62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="G13" s="62">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="H13" s="62">
+        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="I13" s="62">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
+      <c r="J13" s="62">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="K13" s="64"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="55">
+        <f>SUM(M5:M9)</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="55">
+        <f>SUM(C11:J11)</f>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="59" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="59" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K34" s="10"/>
+    </row>
+    <row r="35" spans="2:11" ht="18" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="G35" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="H35" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="I35" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="J35" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="K35" s="11"/>
+    </row>
+    <row r="36" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="48">
+        <v>1</v>
+      </c>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="48">
+        <v>1</v>
+      </c>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="49">
+        <v>1</v>
+      </c>
+      <c r="K36" s="63"/>
+    </row>
+    <row r="37" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39">
+        <v>1</v>
+      </c>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="41"/>
+      <c r="K37" s="63"/>
+    </row>
+    <row r="38" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39">
+        <v>1</v>
+      </c>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="63"/>
+    </row>
+    <row r="39" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39">
+        <v>1</v>
+      </c>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="41"/>
+      <c r="K39" s="63"/>
+    </row>
+    <row r="40" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40">
+        <v>1</v>
+      </c>
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="63"/>
+    </row>
+    <row r="41" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:11" ht="18" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="50">
+        <v>25</v>
+      </c>
+      <c r="D42" s="50">
+        <v>25</v>
+      </c>
+      <c r="E42" s="50">
+        <v>30</v>
+      </c>
+      <c r="F42" s="50">
+        <v>60</v>
+      </c>
+      <c r="G42" s="50">
+        <v>80</v>
+      </c>
+      <c r="H42" s="50">
+        <v>85</v>
+      </c>
+      <c r="I42" s="50">
+        <v>100</v>
+      </c>
+      <c r="J42" s="50">
+        <v>50</v>
+      </c>
+      <c r="K42" s="60"/>
+    </row>
+    <row r="43" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:11" ht="18" outlineLevel="1" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f>C42 * SUM(C36:C40)</f>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Marginal cost model finished
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 03/AMPL Models/Model Setup.xlsx
+++ b/03 - Homework/HW 03/AMPL Models/Model Setup.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/03 - Homework/HW 03/AMPL Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1326" documentId="8_{F9186C4A-4D24-4C11-A94A-4E97A374E8E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8CFD45CF-6228-4D09-86EC-29854484109D}"/>
+  <xr:revisionPtr revIDLastSave="1579" documentId="8_{F9186C4A-4D24-4C11-A94A-4E97A374E8E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F85856A5-B00A-449C-8FA4-85BB01863598}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2581705E-783A-44E8-BFE7-0D5AB3EE4BE1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2581705E-783A-44E8-BFE7-0D5AB3EE4BE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem 1" sheetId="1" r:id="rId1"/>
     <sheet name="Problem 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Problem 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="129">
   <si>
     <t>A</t>
   </si>
@@ -1328,19 +1329,115 @@
   </si>
   <si>
     <t>Actual</t>
+  </si>
+  <si>
+    <t>WII</t>
+  </si>
+  <si>
+    <t>WRS</t>
+  </si>
+  <si>
+    <t>WE</t>
+  </si>
+  <si>
+    <t>WU</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>s in SUPPLIERS</t>
+  </si>
+  <si>
+    <t>WOW</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Demand Parameter</t>
+  </si>
+  <si>
+    <t>Decisions</t>
+  </si>
+  <si>
+    <t>Marginal Cost</t>
+  </si>
+  <si>
+    <t>MC, if buy from WRS</t>
+  </si>
+  <si>
+    <t>MC, if not buy from WII</t>
+  </si>
+  <si>
+    <t>Fixed Fee if Used</t>
+  </si>
+  <si>
+    <t>MC, if purchase 15,000, else not available</t>
+  </si>
+  <si>
+    <t>MC first 3,000</t>
+  </si>
+  <si>
+    <t>MC 3,000-9,000</t>
+  </si>
+  <si>
+    <t>MC &gt;9,000</t>
+  </si>
+  <si>
+    <t>Marginal Only</t>
+  </si>
+  <si>
+    <t>Above</t>
+  </si>
+  <si>
+    <t>Sum of all widgets equal to demand (do a for loop later)</t>
+  </si>
+  <si>
+    <t>Piecewise</t>
+  </si>
+  <si>
+    <t>Fixed cost</t>
+  </si>
+  <si>
+    <t>Either or</t>
+  </si>
+  <si>
+    <t>Rstricted set or range</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Piece 1</t>
+  </si>
+  <si>
+    <t>Piece 2</t>
+  </si>
+  <si>
+    <t>Piece 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0&quot; tons&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0&quot; widgets&quot;"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1535,8 +1632,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1628,6 +1732,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2007,12 +2117,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="13" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2135,8 +2246,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="12" borderId="21" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="13" fillId="12" borderId="21" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="13" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="14" fillId="13" borderId="22" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
@@ -3010,8 +3172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71F040E-57EE-4CA4-8D4D-1306A72BE7E8}">
   <dimension ref="B1:L63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -3731,4 +3893,308 @@
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E494735-2DB7-4BC9-BFC0-578E86A6BACF}">
+  <dimension ref="A2:M29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="28"/>
+    <col min="2" max="6" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="66">
+        <v>17999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="63"/>
+      <c r="D4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="72" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="54"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+    </row>
+    <row r="8" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="75" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <f>A6 + 1</f>
+        <v>1</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="22">
+        <v>18000</v>
+      </c>
+      <c r="D9" s="67">
+        <v>4.95</v>
+      </c>
+      <c r="G9" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="83">
+        <f>D9 * D2</f>
+        <v>89095.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="46"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="67"/>
+    </row>
+    <row r="11" spans="1:10" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="76"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="75" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="28">
+        <f>A9 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="22">
+        <v>14000</v>
+      </c>
+      <c r="D12" s="68">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E12" s="74">
+        <v>20000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="74"/>
+    </row>
+    <row r="14" spans="1:10" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="76"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="78" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="75" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="28">
+        <f>A12 + 1</f>
+        <v>3</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="22">
+        <v>7000</v>
+      </c>
+      <c r="D15" s="68">
+        <v>3.95</v>
+      </c>
+      <c r="E15" s="68">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="79"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="80"/>
+    </row>
+    <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B17" s="79"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="80"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="28">
+        <f>A15 + 1</f>
+        <v>4</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="22">
+        <v>22000</v>
+      </c>
+      <c r="D18" s="69">
+        <v>4.25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="62"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="69"/>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="79"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="78" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="81" t="s">
+        <v>116</v>
+      </c>
+      <c r="F20" s="75" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" t="s">
+        <v>106</v>
+      </c>
+      <c r="J20" s="65">
+        <f>D2</f>
+        <v>17999</v>
+      </c>
+      <c r="K20" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="L20" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="M20" s="73" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="28">
+        <f t="shared" ref="A21" si="0">A18 + 1</f>
+        <v>5</v>
+      </c>
+      <c r="B21" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="22">
+        <v>25000</v>
+      </c>
+      <c r="D21" s="69">
+        <v>9.5</v>
+      </c>
+      <c r="E21" s="69">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F21" s="69">
+        <v>2.75</v>
+      </c>
+      <c r="G21" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="82">
+        <f>SUMPRODUCT(K21:M21, D21:F21)</f>
+        <v>82647.25</v>
+      </c>
+      <c r="K21">
+        <f>IF(J20 &gt;= 3000, 3000, J20)</f>
+        <v>3000</v>
+      </c>
+      <c r="L21">
+        <f>IF(AND(J20 &gt;= 3000, J20 &lt;= 9000), J20 - K21, IF(K21 &lt;&gt; J20, 9000 - K21, 0))</f>
+        <v>6000</v>
+      </c>
+      <c r="M21">
+        <f>IF(J20 &gt;= 9000, J20 - SUM(K21:L21), 0)</f>
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="15" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial go at p3 math formulatioin
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 03/AMPL Models/Model Setup.xlsx
+++ b/03 - Homework/HW 03/AMPL Models/Model Setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/03 - Homework/HW 03/AMPL Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1579" documentId="8_{F9186C4A-4D24-4C11-A94A-4E97A374E8E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F85856A5-B00A-449C-8FA4-85BB01863598}"/>
+  <xr:revisionPtr revIDLastSave="1710" documentId="8_{F9186C4A-4D24-4C11-A94A-4E97A374E8E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{43AEF3E6-F98B-42A3-9E3C-EF9D76F2F644}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2581705E-783A-44E8-BFE7-0D5AB3EE4BE1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="137">
   <si>
     <t>A</t>
   </si>
@@ -1355,9 +1355,6 @@
     <t>Available</t>
   </si>
   <si>
-    <t>Demand</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -1409,9 +1406,6 @@
     <t>Either or</t>
   </si>
   <si>
-    <t>Rstricted set or range</t>
-  </si>
-  <si>
     <t>Simple</t>
   </si>
   <si>
@@ -1422,6 +1416,36 @@
   </si>
   <si>
     <t>Piece 3</t>
+  </si>
+  <si>
+    <t>Marginal</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Model Examples</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Rstricted range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if WRS, then either WE or WII: </t>
+  </si>
+  <si>
+    <t>MC 1</t>
+  </si>
+  <si>
+    <t>MC2</t>
+  </si>
+  <si>
+    <t>WE2</t>
+  </si>
+  <si>
+    <t>WE1</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1459,7 @@
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0&quot; tons&quot;"/>
     <numFmt numFmtId="167" formatCode="#,##0&quot; widgets&quot;"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25" x14ac:knownFonts="1">
     <font>
@@ -1742,7 +1766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -2116,6 +2140,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2123,7 +2156,7 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2260,8 +2293,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2290,12 +2323,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="14" fillId="13" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="14" fillId="13" borderId="22" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="43" fontId="14" fillId="13" borderId="22" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="13" fillId="12" borderId="21" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -3897,30 +3939,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E494735-2DB7-4BC9-BFC0-578E86A6BACF}">
-  <dimension ref="A2:M29"/>
+  <dimension ref="A2:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="28"/>
     <col min="2" max="6" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="2.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C2" s="64" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="66">
+        <v>5000</v>
+      </c>
+      <c r="L2" s="90" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" s="90" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="83">
+        <f>SUM($L$9,L$12,$L$15,$L$18,$L$21)</f>
+        <v>364350</v>
+      </c>
+      <c r="M3" s="83">
+        <f>SUM($L$9,M$12,$L$15,$L$18,$L$21)</f>
+        <v>344350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="70" t="s">
         <v>108</v>
-      </c>
-      <c r="D2" s="66">
-        <v>17999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="70" t="s">
-        <v>109</v>
       </c>
       <c r="C4" s="63"/>
       <c r="D4" s="16" t="s">
@@ -3930,7 +3996,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="71" t="s">
         <v>102</v>
       </c>
@@ -3942,7 +4008,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="72" t="s">
         <v>103</v>
       </c>
@@ -3951,13 +4017,21 @@
       <c r="E6" s="45"/>
       <c r="F6" s="45"/>
       <c r="G6" s="45"/>
-    </row>
-    <row r="8" spans="1:10" s="75" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="87" t="s">
+        <v>129</v>
+      </c>
+      <c r="K6" s="87"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+    </row>
+    <row r="8" spans="1:16" s="75" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="75" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <f>A6 + 1</f>
         <v>1</v>
@@ -3972,32 +4046,45 @@
         <v>4.95</v>
       </c>
       <c r="G9" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="83">
-        <f>D9 * D2</f>
-        <v>89095.05</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="65">
+        <f>C9</f>
+        <v>18000</v>
+      </c>
+      <c r="L9" s="83">
+        <f>IF($K$9 &lt;= C9, D9 * $K$9, 0)</f>
+        <v>89100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="46"/>
       <c r="C10" s="22"/>
       <c r="D10" s="67"/>
     </row>
-    <row r="11" spans="1:10" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="76"/>
       <c r="C11" s="77"/>
       <c r="D11" s="78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E11" s="75" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="L11" s="75" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="75" t="s">
+        <v>127</v>
+      </c>
+      <c r="N11" s="75" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <f>A9 + 1</f>
         <v>2</v>
@@ -4015,26 +4102,51 @@
         <v>20000</v>
       </c>
       <c r="G12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="65">
+        <f>C12</f>
+        <v>14000</v>
+      </c>
+      <c r="L12" s="85">
+        <f>IF($K$12 &lt;= C12, SUM(M12:N12), 0)</f>
+        <v>52200</v>
+      </c>
+      <c r="M12" s="84">
+        <f>D12 * $K$12</f>
+        <v>32199.999999999996</v>
+      </c>
+      <c r="N12" s="84">
+        <f>IF(K12 &gt; 0, E12, 0)</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="22"/>
       <c r="D13" s="68"/>
       <c r="E13" s="74"/>
     </row>
-    <row r="14" spans="1:10" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="76"/>
       <c r="C14" s="77"/>
       <c r="D14" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="75" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L14" s="75" t="s">
+        <v>133</v>
+      </c>
+      <c r="M14" s="75" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <f>A12 + 1</f>
         <v>3</v>
@@ -4052,24 +4164,42 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="G15" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="K15" s="65">
+        <f>C15</f>
+        <v>7000</v>
+      </c>
+      <c r="L15" s="89">
+        <f>D15 * $K$15</f>
+        <v>27650</v>
+      </c>
+      <c r="M15" s="89">
+        <f>E15 * $K$15</f>
+        <v>28699.999999999996</v>
+      </c>
+      <c r="P15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="79"/>
       <c r="C16" s="22"/>
       <c r="D16" s="80"/>
       <c r="E16" s="80"/>
     </row>
-    <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="79"/>
       <c r="C17" s="22"/>
       <c r="D17" s="78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" s="80"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="73" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="28">
         <f>A15 + 1</f>
         <v>4</v>
@@ -4084,44 +4214,51 @@
         <v>4.25</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="65">
+        <f>C18</f>
+        <v>22000</v>
+      </c>
+      <c r="L18" s="82">
+        <f>IF($K$18 &lt;= C18, IF(K18 &lt; M18, 0, D18 * K18), 0)</f>
+        <v>93500</v>
+      </c>
+      <c r="M18" s="88">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="62"/>
       <c r="C19" s="22"/>
       <c r="D19" s="69"/>
     </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="79"/>
       <c r="C20" s="22"/>
       <c r="D20" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="E20" s="81" t="s">
+      <c r="F20" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="75" t="s">
-        <v>117</v>
-      </c>
-      <c r="I20" t="s">
-        <v>106</v>
-      </c>
-      <c r="J20" s="65">
-        <f>D2</f>
-        <v>17999</v>
-      </c>
-      <c r="K20" s="73" t="s">
+      <c r="M20" s="73" t="s">
+        <v>124</v>
+      </c>
+      <c r="N20" s="73" t="s">
+        <v>125</v>
+      </c>
+      <c r="O20" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="L20" s="73" t="s">
-        <v>127</v>
-      </c>
-      <c r="M20" s="73" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="28">
         <f t="shared" ref="A21" si="0">A18 + 1</f>
         <v>5</v>
@@ -4142,54 +4279,58 @@
         <v>2.75</v>
       </c>
       <c r="G21" t="s">
-        <v>121</v>
-      </c>
-      <c r="I21" t="s">
+        <v>120</v>
+      </c>
+      <c r="J21" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="82">
-        <f>SUMPRODUCT(K21:M21, D21:F21)</f>
-        <v>82647.25</v>
-      </c>
-      <c r="K21">
-        <f>IF(J20 &gt;= 3000, 3000, J20)</f>
+      <c r="K21" s="65">
+        <f>C21</f>
+        <v>25000</v>
+      </c>
+      <c r="L21" s="82">
+        <f>IF($K$21 &lt;= C21, SUMPRODUCT(M21:O21, D21:F21), 0)</f>
+        <v>101900</v>
+      </c>
+      <c r="M21">
+        <f>IF($K$21 &gt;= 3000, 3000, $K$21)</f>
         <v>3000</v>
       </c>
-      <c r="L21">
-        <f>IF(AND(J20 &gt;= 3000, J20 &lt;= 9000), J20 - K21, IF(K21 &lt;&gt; J20, 9000 - K21, 0))</f>
+      <c r="N21">
+        <f>IF(AND($K$21 &gt;= 3000, $K$21 &lt;= 9000), $K$21 - M21, IF(M21 &lt;&gt; $K$21, 9000 - M21, 0))</f>
         <v>6000</v>
       </c>
-      <c r="M21">
-        <f>IF(J20 &gt;= 9000, J20 - SUM(K21:L21), 0)</f>
-        <v>8999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <f>IF($K$21 &gt;= 9000, $K$21 - SUM(M21:N21), 0)</f>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>